<commit_message>
update to reflect beta #1
</commit_message>
<xml_diff>
--- a/Branches/2.0/doc/iResearch Version 2.0 - Beta #1.xlsx
+++ b/Branches/2.0/doc/iResearch Version 2.0 - Beta #1.xlsx
@@ -16,11 +16,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="40">
   <si>
     <t>Feature</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
     <t>2.       You can see examples of the charts and tables etc in the note names Flashnote.</t>
   </si>
   <si>
@@ -69,13 +72,37 @@
     <t>19.   The note will be the same size and font of the source, analysts should be able to add this along with a superscript note in the headline of the table.</t>
   </si>
   <si>
-    <t>20.   In charts, there will be no gridlines and legends will appear at the bottom.</t>
-  </si>
-  <si>
     <t>21.   The headlines of charts will be like the tables, with a line above and below, same text size, line point spacing, bolding. They will also have a line below a source under just like in tables.</t>
   </si>
   <si>
     <t>22.   Analysts should be able to add a single chart, stretched all the way to the other side of the page with solid lines above and below, or two charts with a separator in the lines which I have done by adding a column between them that has no borders.</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Insert</t>
+  </si>
+  <si>
+    <t>Tables</t>
+  </si>
+  <si>
+    <t>Charts</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>adjust fields</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
   <si>
     <t>1.       The reports we will need are: flashnote, company update, initiation, sector note, macro and strategy report. 
@@ -97,14 +124,35 @@
          You will see the same before the Note in that column. </t>
   </si>
   <si>
-    <t>iResearch Version 2.0 - Beta #1</t>
+    <t>iResearch Version 2.0</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23. Use same margins for all pages </t>
+  </si>
+  <si>
+    <t xml:space="preserve">24. Having Text Sections inside a layout table </t>
+  </si>
+  <si>
+    <t>25. Start page number from 2 not 1</t>
+  </si>
+  <si>
+    <t>26. Use the updated logo</t>
+  </si>
+  <si>
+    <t>27. Desclaimer font is 11 not 8</t>
+  </si>
+  <si>
+    <t>20.   In charts, there will be no gridlines and no legend for now</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +181,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -154,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -166,11 +226,92 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -231,10 +372,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:B25" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="B3:B25"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Feature" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:F30" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="B3:F30">
+    <filterColumn colId="2">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="B4:F30">
+    <sortCondition ref="F3:F30"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Feature" dataDxfId="4"/>
+    <tableColumn id="2" name="Component" dataDxfId="3"/>
+    <tableColumn id="3" name="Status" dataDxfId="2"/>
+    <tableColumn id="4" name="Comments" dataDxfId="1"/>
+    <tableColumn id="5" name="#" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -525,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:B25"/>
+  <dimension ref="B1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -539,124 +693,423 @@
     <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75">
+    <row r="1" spans="2:6" ht="18.75">
       <c r="B1" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:2" ht="51">
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="51">
       <c r="B4" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2">
+        <v>29</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" hidden="1">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:2">
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="2:2">
+      <c r="C6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="2:2" ht="25.5">
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="2:2">
+      <c r="C8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="25.5">
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="2:2" ht="25.5">
+      <c r="C9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="2:2" ht="38.25">
+      <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="25.5">
       <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="38.25">
+      <c r="B12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="89.25">
+      <c r="B13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="25.5">
+      <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="25.5">
+      <c r="B15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="38.25" hidden="1">
+      <c r="B17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" hidden="1">
+      <c r="B18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" hidden="1">
+      <c r="B19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="25.5" hidden="1">
+      <c r="B20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="25.5">
+      <c r="B21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="25.5">
+      <c r="B22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="25.5">
+      <c r="B24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="5">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:2" ht="89.25">
-      <c r="B12" s="3" t="s">
+    <row r="25" spans="2:6" ht="25.5">
+      <c r="B25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="5">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="2:2">
-      <c r="B13" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2">
-      <c r="B14" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2" ht="25.5">
-      <c r="B15" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2" ht="25.5">
-      <c r="B16" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" ht="25.5">
-      <c r="B17" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" ht="25.5">
-      <c r="B18" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" ht="38.25">
-      <c r="B19" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" ht="25.5">
-      <c r="B22" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" ht="25.5">
-      <c r="B24" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" ht="25.5">
-      <c r="B25" s="3" t="s">
-        <v>16</v>
+    <row r="26" spans="2:6">
+      <c r="B26" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="B29" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>